<commit_message>
remove disc per from UI, bhp and mileage from upload
</commit_message>
<xml_diff>
--- a/server/apis/bulkUpload/SampleTemplate/Records.xlsx
+++ b/server/apis/bulkUpload/SampleTemplate/Records.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -61,13 +61,7 @@
     <t xml:space="preserve">cc</t>
   </si>
   <si>
-    <t xml:space="preserve">bhp</t>
-  </si>
-  <si>
     <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mileage</t>
   </si>
   <si>
     <t xml:space="preserve">images</t>
@@ -212,10 +206,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -233,15 +227,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="39.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="20" style="1" width="8.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1022" style="1" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="39.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="20.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="18" style="1" width="8.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1020" style="1" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,76 +282,64 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>27</v>
+      <c r="P2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>